<commit_message>
Review and correction of all Forms. Notes in FormNotes.xlsx. Review and edits to RSM as well to fix font mismatch, list of effective pages, acronyms list. Major edit
</commit_message>
<xml_diff>
--- a/FM/FormNamingConventions.xlsx
+++ b/FM/FormNamingConventions.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/croe10/workspace/RepairServiceManual/FM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60F12BDD-4545-DE44-B2B7-E0BE2A61396B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989BAA96-B6BE-F943-B860-FB4874B0716A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17980" yWindow="9060" windowWidth="28040" windowHeight="17440" xr2:uid="{7075392B-EF23-6049-9CE0-8C0DA18CC28E}"/>
+    <workbookView xWindow="108020" yWindow="-3200" windowWidth="32160" windowHeight="17440" activeTab="1" xr2:uid="{7075392B-EF23-6049-9CE0-8C0DA18CC28E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="249">
   <si>
     <t>AA-ACT</t>
   </si>
@@ -418,13 +420,367 @@
   </si>
   <si>
     <t>- Totally sub numbers</t>
+  </si>
+  <si>
+    <t>Form/Tag/</t>
+  </si>
+  <si>
+    <t>A-ACT</t>
+  </si>
+  <si>
+    <t>Long Name</t>
+  </si>
+  <si>
+    <t>AirSpeed Calibration/Test</t>
+  </si>
+  <si>
+    <t>Form Updated</t>
+  </si>
+  <si>
+    <t>PDF Produced</t>
+  </si>
+  <si>
+    <t>Forms Manual Updated</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>PDF FORM?</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Comments/Notes</t>
+  </si>
+  <si>
+    <t>A-AT</t>
+  </si>
+  <si>
+    <t>A-ATC-TMSI</t>
+  </si>
+  <si>
+    <t>A-ATCC</t>
+  </si>
+  <si>
+    <t>A-ATI</t>
+  </si>
+  <si>
+    <t>A-AWBR</t>
+  </si>
+  <si>
+    <t>A-CC</t>
+  </si>
+  <si>
+    <t>A-CL</t>
+  </si>
+  <si>
+    <t>A-CLSE</t>
+  </si>
+  <si>
+    <t>A-CSDS</t>
+  </si>
+  <si>
+    <t>A-ECTCR</t>
+  </si>
+  <si>
+    <t>A-ETR</t>
+  </si>
+  <si>
+    <t>A-IIC</t>
+  </si>
+  <si>
+    <t>A-MACS</t>
+  </si>
+  <si>
+    <t>A-MCR</t>
+  </si>
+  <si>
+    <t>A-RT</t>
+  </si>
+  <si>
+    <t>A-RTL</t>
+  </si>
+  <si>
+    <t>A-SPL</t>
+  </si>
+  <si>
+    <t>A-TECIF</t>
+  </si>
+  <si>
+    <t>A-VSICC</t>
+  </si>
+  <si>
+    <t>A-WO</t>
+  </si>
+  <si>
+    <t>A-WOC</t>
+  </si>
+  <si>
+    <t>AA-AFCA</t>
+  </si>
+  <si>
+    <t>AA-AFCL</t>
+  </si>
+  <si>
+    <t>AA-AR</t>
+  </si>
+  <si>
+    <t>AA-CVA</t>
+  </si>
+  <si>
+    <t>AA-IA</t>
+  </si>
+  <si>
+    <t>AA-VA</t>
+  </si>
+  <si>
+    <t>AL-ACMR</t>
+  </si>
+  <si>
+    <t>AL-ATI</t>
+  </si>
+  <si>
+    <t>AL-GAMR</t>
+  </si>
+  <si>
+    <t>Autopilot Test</t>
+  </si>
+  <si>
+    <t>FileNames Updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not included in Forms manual. Should we add? </t>
+  </si>
+  <si>
+    <t>ATC Transponder and Mode S Inspection</t>
+  </si>
+  <si>
+    <t>Aircraft Task Completion Checklist</t>
+  </si>
+  <si>
+    <t>Altimeter Test/Inspection</t>
+  </si>
+  <si>
+    <t>Aircraft Weight and Balance Revision</t>
+  </si>
+  <si>
+    <t>Original PDF Form from Kings - can be improved. NOT exhaustively tested or reviewed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AD-Toolbox PDF form, modified with Alta Avionics Logo etc. </t>
+  </si>
+  <si>
+    <t>Excel spreadsheet</t>
+  </si>
+  <si>
+    <t>Certificate of Calibration</t>
+  </si>
+  <si>
+    <t>Calibration List</t>
+  </si>
+  <si>
+    <t>Not included in Forms manual. Should we add? Already being used. Need to fix font size on list</t>
+  </si>
+  <si>
+    <t>Capabilities List Self Evaluation Form</t>
+  </si>
+  <si>
+    <t>Could be made into PDF form if desired.</t>
+  </si>
+  <si>
+    <t>Compass Swing Documentation Sheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electromagnetic Compatibility Test Completion Record </t>
+  </si>
+  <si>
+    <t>Employee Training Record</t>
+  </si>
+  <si>
+    <t>Installation Inspection Checklist</t>
+  </si>
+  <si>
+    <t>Master Altimeter Correction Sheet</t>
+  </si>
+  <si>
+    <t>Manual Change Request</t>
+  </si>
+  <si>
+    <t>Radar Test</t>
+  </si>
+  <si>
+    <t>Required Training Log</t>
+  </si>
+  <si>
+    <t>Scrapped Parts Log</t>
+  </si>
+  <si>
+    <t>Should this actually be included in the Forms Manual? Other log (eg. Calibration are not)</t>
+  </si>
+  <si>
+    <t>Test Equipment Calibration and Inspection Form</t>
+  </si>
+  <si>
+    <t>Vertical Speed Indicator Correction Card</t>
+  </si>
+  <si>
+    <t>Work Order</t>
+  </si>
+  <si>
+    <t>Work Order Continuation</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Audit Findings / Corrective Action</t>
+  </si>
+  <si>
+    <t>This is the one with underlines under the checkmarks. Missing instructions. May have further changes from Jeff and Rita.</t>
+  </si>
+  <si>
+    <t>This has yet to be produced. Will Probably be PDF form</t>
+  </si>
+  <si>
+    <t>Audit Findings Control Log</t>
+  </si>
+  <si>
+    <t>Audit Request</t>
+  </si>
+  <si>
+    <t>Calibrated Vendor Audit</t>
+  </si>
+  <si>
+    <t>Internal Audit</t>
+  </si>
+  <si>
+    <t>Vendor Audit</t>
+  </si>
+  <si>
+    <t>Air Carrier Maintenance Release</t>
+  </si>
+  <si>
+    <t>No Instructions for filing out form?</t>
+  </si>
+  <si>
+    <t>Altimeter Test and Inspection</t>
+  </si>
+  <si>
+    <t>Make this a PDF Form? Do we have to do this before FM manual submission?</t>
+  </si>
+  <si>
+    <t>General Aviation Maintenance Release</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>AT-C</t>
+  </si>
+  <si>
+    <t>AT-DNF</t>
+  </si>
+  <si>
+    <t>AT-LS</t>
+  </si>
+  <si>
+    <t>AT-MC</t>
+  </si>
+  <si>
+    <t>AT-RAS</t>
+  </si>
+  <si>
+    <t>AT-RFS</t>
+  </si>
+  <si>
+    <t>AT-RI</t>
+  </si>
+  <si>
+    <t>AT-S</t>
+  </si>
+  <si>
+    <t>AT-T43</t>
+  </si>
+  <si>
+    <t>AT-W</t>
+  </si>
+  <si>
+    <t>Calibration Sticker</t>
+  </si>
+  <si>
+    <t>DO NOT FLY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avery label word doc exists but is ths what we want to use for this? </t>
+  </si>
+  <si>
+    <t>Locator Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual Correct </t>
+  </si>
+  <si>
+    <t>Removed As Servicable</t>
+  </si>
+  <si>
+    <t>CRS Number needs to be changed. I don't have the original, just a scan of the tag.</t>
+  </si>
+  <si>
+    <t>AT-REP</t>
+  </si>
+  <si>
+    <t>Repairable Equipment Part</t>
+  </si>
+  <si>
+    <t>CRS Number needs to be changed. I don't have the original, just a scan of the tag. This is a new tag to me. Where did this come from?</t>
+  </si>
+  <si>
+    <t>Removed for Storage</t>
+  </si>
+  <si>
+    <t>Rejected Item</t>
+  </si>
+  <si>
+    <t>no Instructions for filing out form? Should this be labelled 'Removed for Storage"?</t>
+  </si>
+  <si>
+    <t>Scrap</t>
+  </si>
+  <si>
+    <t>AT-SLI</t>
+  </si>
+  <si>
+    <t>Shelf Life Item</t>
+  </si>
+  <si>
+    <t>Test As Per FAR 43</t>
+  </si>
+  <si>
+    <t>FAA-8130-3</t>
+  </si>
+  <si>
+    <t>Authorized Release Certificate</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>FAA-337</t>
+  </si>
+  <si>
+    <t>Major Alteration or Repair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not included in Forms manual.  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -435,6 +791,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -461,15 +825,69 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -480,6 +898,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3FB28EC-4342-0740-9F16-BE0412193862}" name="Table1" displayName="Table1" ref="B1:I43" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3">
+  <autoFilter ref="B1:I43" xr:uid="{714A178E-D64B-314B-B9B3-3D09EA0AF3D7}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{32986FBA-C172-A043-85F3-7E0818FEEE68}" name="Form/Tag/"/>
+    <tableColumn id="2" xr3:uid="{38CD2EF5-260C-6642-9281-DFC3A818E877}" name="Long Name"/>
+    <tableColumn id="3" xr3:uid="{E0333E3D-B6F5-E349-A36A-6FCE18153F6E}" name="Form Updated" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{0F863359-1ACA-9D41-B965-35E38CCF86E8}" name="FileNames Updated" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{80EB687D-D24B-3743-B86E-F5772B7FF303}" name="PDF Produced" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{C6A1CC92-CF0D-924D-AD57-B6180B97DB1A}" name="PDF FORM?" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{73F27AB8-0834-5A44-AE3E-05D66B13CCE8}" name="Forms Manual Updated" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{06E97318-41ED-B84E-8966-E579096B7360}" name="Comments/Notes" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -781,14 +1216,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35085BFF-374C-3240-8BDC-782CDF4506C6}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.6640625" customWidth="1"/>
     <col min="2" max="4" width="29" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1302,4 +1738,1341 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A72881F-73D1-5048-B787-E23100BF1C70}">
+  <dimension ref="A1:I46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="22.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="76" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f t="shared" ref="A4:A43" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>146</v>
+      </c>
+      <c r="C6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" t="s">
+        <v>182</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" t="s">
+        <v>185</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" t="s">
+        <v>188</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C12" t="s">
+        <v>190</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" t="s">
+        <v>192</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" t="s">
+        <v>194</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" t="s">
+        <v>198</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" t="s">
+        <v>199</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20" t="s">
+        <v>200</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C21" t="s">
+        <v>202</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" t="s">
+        <v>205</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" t="s">
+        <v>206</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>166</v>
+      </c>
+      <c r="C24" t="s">
+        <v>207</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>167</v>
+      </c>
+      <c r="C25" t="s">
+        <v>208</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>168</v>
+      </c>
+      <c r="C26" t="s">
+        <v>209</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" t="s">
+        <v>210</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>170</v>
+      </c>
+      <c r="C28" t="s">
+        <v>212</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>171</v>
+      </c>
+      <c r="C29" t="s">
+        <v>214</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" t="s">
+        <v>226</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>217</v>
+      </c>
+      <c r="C31" t="s">
+        <v>227</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>218</v>
+      </c>
+      <c r="C32" t="s">
+        <v>229</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>219</v>
+      </c>
+      <c r="C33" t="s">
+        <v>230</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>220</v>
+      </c>
+      <c r="C34" t="s">
+        <v>231</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>233</v>
+      </c>
+      <c r="C35" t="s">
+        <v>234</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>221</v>
+      </c>
+      <c r="C36" t="s">
+        <v>236</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>222</v>
+      </c>
+      <c r="C37" t="s">
+        <v>237</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>223</v>
+      </c>
+      <c r="C38" t="s">
+        <v>239</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>240</v>
+      </c>
+      <c r="C39" t="s">
+        <v>241</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>224</v>
+      </c>
+      <c r="C40" t="s">
+        <v>242</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>225</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>246</v>
+      </c>
+      <c r="C42" t="s">
+        <v>247</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>243</v>
+      </c>
+      <c r="C43" t="s">
+        <v>244</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" t="s">
+        <v>172</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>148</v>
+      </c>
+      <c r="C45" t="s">
+        <v>183</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46" t="s">
+        <v>193</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>